<commit_message>
updated Career knowwledge file
</commit_message>
<xml_diff>
--- a/Common/PL file/Career Knowledge_Latest.xlsx
+++ b/Common/PL file/Career Knowledge_Latest.xlsx
@@ -9224,6 +9224,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -9231,9 +9237,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -9249,6 +9252,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="38" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -9273,36 +9303,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -9353,6 +9353,30 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="25" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="25" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="25" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="25" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="25" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="25" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="25" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="25" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -9380,12 +9404,6 @@
     <xf numFmtId="0" fontId="36" fillId="25" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="25" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="25" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="25" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -9396,24 +9414,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="25" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="25" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="25" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="25" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="25" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="25" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="25" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -11082,7 +11082,7 @@
   <dimension ref="A1:V209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11126,18 +11126,18 @@
     <row r="2" spans="4:20" ht="21" x14ac:dyDescent="0.35">
       <c r="E2" s="266">
         <f ca="1">TODAY()</f>
-        <v>43293</v>
+        <v>43294</v>
       </c>
       <c r="F2" s="266">
         <v>43621</v>
       </c>
       <c r="G2" s="267">
         <f ca="1">DATEDIF(E2,F2,"d")</f>
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H2" s="267">
         <f ca="1">(DATEDIF(E2,F2,"d")/7)</f>
-        <v>46.857142857142854</v>
+        <v>46.714285714285715</v>
       </c>
       <c r="I2" s="267">
         <f ca="1">DATEDIF(E2,F2,"m")</f>
@@ -11179,7 +11179,7 @@
       <c r="J5" s="90"/>
       <c r="K5" s="192">
         <f>P5</f>
-        <v>30.68</v>
+        <v>30.26</v>
       </c>
       <c r="L5" s="309">
         <f>(L6/64)</f>
@@ -11191,11 +11191,11 @@
       <c r="N5" s="329"/>
       <c r="O5" s="295">
         <f>SUM(G7:G9,G13,G18:G24)</f>
-        <v>21721</v>
+        <v>21421</v>
       </c>
       <c r="P5" s="192">
         <f>ROUND((O5/O6)*100,2)</f>
-        <v>30.68</v>
+        <v>30.26</v>
       </c>
     </row>
     <row r="6" spans="4:20" x14ac:dyDescent="0.25">
@@ -11275,11 +11275,11 @@
       </c>
       <c r="S7" s="5">
         <f>(O8*64)</f>
-        <v>201216</v>
+        <v>171200</v>
       </c>
       <c r="T7" s="291">
         <f>(SUM(S6:S7))</f>
-        <v>392960</v>
+        <v>362944</v>
       </c>
     </row>
     <row r="8" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11311,18 +11311,18 @@
       <c r="N8" s="331"/>
       <c r="O8" s="298">
         <f>G14</f>
-        <v>3144</v>
+        <v>2675</v>
       </c>
       <c r="R8" s="290" t="s">
         <v>1850</v>
       </c>
       <c r="S8" s="5">
         <f>(O5*64)</f>
-        <v>1390144</v>
+        <v>1370944</v>
       </c>
       <c r="T8" s="291">
         <f>S8</f>
-        <v>1390144</v>
+        <v>1370944</v>
       </c>
     </row>
     <row r="9" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11361,7 +11361,7 @@
       <c r="N9" s="332"/>
       <c r="O9" s="116">
         <f>SUM(O5,O7,O8)</f>
-        <v>27861</v>
+        <v>27092</v>
       </c>
       <c r="R9" s="292" t="s">
         <v>1851</v>
@@ -11371,7 +11371,7 @@
       </c>
       <c r="T9" s="294">
         <f>SUM(T7,T8,S9)</f>
-        <v>1983104</v>
+        <v>1933888</v>
       </c>
     </row>
     <row r="10" spans="4:20" ht="31.5" x14ac:dyDescent="0.5">
@@ -11420,14 +11420,14 @@
         <v>141</v>
       </c>
       <c r="G13" s="86">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="H13" s="121">
         <v>3500</v>
       </c>
       <c r="I13" s="114">
         <f>(G13/H13)*100</f>
-        <v>8.5714285714285712</v>
+        <v>0</v>
       </c>
       <c r="J13" s="121">
         <v>11.75</v>
@@ -11441,7 +11441,7 @@
         <v>758</v>
       </c>
       <c r="G14" s="86">
-        <v>3144</v>
+        <v>2675</v>
       </c>
       <c r="H14" s="121"/>
       <c r="I14" s="114"/>
@@ -11614,7 +11614,7 @@
       </c>
       <c r="L21" s="6">
         <f>ROUND(AVERAGE(I7:I19),2)</f>
-        <v>22.21</v>
+        <v>20.78</v>
       </c>
       <c r="M21" s="6">
         <v>65.44</v>
@@ -11749,11 +11749,11 @@
       </c>
       <c r="G27" s="84">
         <f>SUM(G7:G25)</f>
-        <v>27861</v>
+        <v>27092</v>
       </c>
       <c r="H27" s="268">
         <f>(G27*D27)</f>
-        <v>1763601.2999999998</v>
+        <v>1714923.5999999999</v>
       </c>
       <c r="I27" s="269">
         <f>SUM(G18:G19)</f>
@@ -11761,7 +11761,7 @@
       </c>
       <c r="J27" s="269">
         <f>SUM(G27,-I27)</f>
-        <v>25211</v>
+        <v>24442</v>
       </c>
       <c r="K27" s="182">
         <v>42734</v>
@@ -11777,7 +11777,7 @@
       <c r="I28" s="124"/>
       <c r="J28" s="268">
         <f>(J27*D27)</f>
-        <v>1595856.2999999998</v>
+        <v>1547178.5999999999</v>
       </c>
       <c r="K28" s="182">
         <v>42750</v>
@@ -12405,7 +12405,7 @@
       </c>
       <c r="M58">
         <f>P5</f>
-        <v>30.68</v>
+        <v>30.26</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
@@ -12442,22 +12442,22 @@
       <c r="N64" s="312"/>
     </row>
     <row r="65" spans="2:22" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B65" s="365" t="s">
+      <c r="B65" s="375" t="s">
         <v>1934</v>
       </c>
-      <c r="C65" s="366"/>
-      <c r="F65" s="365" t="s">
+      <c r="C65" s="376"/>
+      <c r="F65" s="375" t="s">
         <v>1780</v>
       </c>
-      <c r="G65" s="366"/>
+      <c r="G65" s="376"/>
       <c r="H65" s="230">
         <f>SUM(G66:G91)</f>
         <v>3439</v>
       </c>
-      <c r="J65" s="365">
+      <c r="J65" s="375">
         <v>43252</v>
       </c>
-      <c r="K65" s="366"/>
+      <c r="K65" s="376"/>
       <c r="L65" s="265">
         <f>SUM(K66:K91)</f>
         <v>-3545</v>
@@ -13878,41 +13878,41 @@
     </row>
     <row r="116" spans="3:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C116" s="245"/>
-      <c r="D116" s="367" t="s">
+      <c r="D116" s="377" t="s">
         <v>1221</v>
       </c>
-      <c r="E116" s="368"/>
-      <c r="F116" s="369"/>
-      <c r="G116" s="370" t="s">
+      <c r="E116" s="378"/>
+      <c r="F116" s="379"/>
+      <c r="G116" s="380" t="s">
         <v>1565</v>
       </c>
-      <c r="H116" s="371"/>
+      <c r="H116" s="381"/>
       <c r="I116" s="199" t="s">
         <v>1566</v>
       </c>
       <c r="J116" s="199" t="s">
         <v>1567</v>
       </c>
-      <c r="K116" s="370" t="s">
+      <c r="K116" s="380" t="s">
         <v>1625</v>
       </c>
-      <c r="L116" s="372"/>
-      <c r="M116" s="371"/>
+      <c r="L116" s="382"/>
+      <c r="M116" s="381"/>
       <c r="N116" s="343"/>
     </row>
     <row r="117" spans="3:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C117" s="245"/>
-      <c r="D117" s="375">
+      <c r="D117" s="366">
         <f>SUM(D115:F115)</f>
         <v>141.49</v>
       </c>
-      <c r="E117" s="376"/>
-      <c r="F117" s="377"/>
-      <c r="G117" s="378">
+      <c r="E117" s="367"/>
+      <c r="F117" s="368"/>
+      <c r="G117" s="369">
         <f>SUM(G115:H115)</f>
         <v>100.53</v>
       </c>
-      <c r="H117" s="379"/>
+      <c r="H117" s="370"/>
       <c r="I117" s="200">
         <f>SUM(I104:I113)</f>
         <v>60.47</v>
@@ -13921,12 +13921,12 @@
         <f>SUM(J104:J113)</f>
         <v>71.55</v>
       </c>
-      <c r="K117" s="380">
+      <c r="K117" s="371">
         <f>SUM(K115:M115)</f>
         <v>166.91000000000003</v>
       </c>
-      <c r="L117" s="381"/>
-      <c r="M117" s="382"/>
+      <c r="L117" s="372"/>
+      <c r="M117" s="373"/>
       <c r="N117" s="344"/>
       <c r="O117" s="1">
         <f>(O115-O103)</f>
@@ -14038,14 +14038,14 @@
         <f>(L124+O120)</f>
         <v>65.62</v>
       </c>
-      <c r="N124" s="356" t="s">
+      <c r="N124" s="358" t="s">
         <v>1221</v>
       </c>
-      <c r="O124" s="356">
+      <c r="O124" s="358">
         <f>SUM(M124:M126)</f>
         <v>149.91</v>
       </c>
-      <c r="P124" s="359">
+      <c r="P124" s="374">
         <f>ROUND(SUM(O124:O133),2)</f>
         <v>564.11</v>
       </c>
@@ -14079,9 +14079,9 @@
         <f>(L125+O120)</f>
         <v>62.819999999999993</v>
       </c>
-      <c r="N125" s="357"/>
-      <c r="O125" s="357"/>
-      <c r="P125" s="359"/>
+      <c r="N125" s="359"/>
+      <c r="O125" s="359"/>
+      <c r="P125" s="374"/>
     </row>
     <row r="126" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C126" t="s">
@@ -14116,9 +14116,9 @@
         <f>(L126+O120)</f>
         <v>21.47</v>
       </c>
-      <c r="N126" s="358"/>
-      <c r="O126" s="358"/>
-      <c r="P126" s="359"/>
+      <c r="N126" s="360"/>
+      <c r="O126" s="360"/>
+      <c r="P126" s="374"/>
     </row>
     <row r="127" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H127" s="5" t="s">
@@ -14143,14 +14143,14 @@
         <f>(L127+O120)</f>
         <v>65.62</v>
       </c>
-      <c r="N127" s="360" t="s">
+      <c r="N127" s="361" t="s">
         <v>1565</v>
       </c>
-      <c r="O127" s="360">
+      <c r="O127" s="361">
         <f>SUM(M127:M128)</f>
         <v>99.95</v>
       </c>
-      <c r="P127" s="359"/>
+      <c r="P127" s="374"/>
     </row>
     <row r="128" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H128" s="5" t="s">
@@ -14174,9 +14174,9 @@
         <f>L128</f>
         <v>34.33</v>
       </c>
-      <c r="N128" s="361"/>
-      <c r="O128" s="361"/>
-      <c r="P128" s="359"/>
+      <c r="N128" s="362"/>
+      <c r="O128" s="362"/>
+      <c r="P128" s="374"/>
     </row>
     <row r="129" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H129" s="5" t="s">
@@ -14208,7 +14208,7 @@
         <f>M129</f>
         <v>62.819999999999993</v>
       </c>
-      <c r="P129" s="359"/>
+      <c r="P129" s="374"/>
     </row>
     <row r="130" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H130" s="5" t="s">
@@ -14240,7 +14240,7 @@
         <f>M130</f>
         <v>75.36999999999999</v>
       </c>
-      <c r="P130" s="359"/>
+      <c r="P130" s="374"/>
     </row>
     <row r="131" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C131">
@@ -14269,14 +14269,14 @@
         <f>(L131+O120)</f>
         <v>72.349999999999994</v>
       </c>
-      <c r="N131" s="362" t="s">
+      <c r="N131" s="363" t="s">
         <v>1983</v>
       </c>
-      <c r="O131" s="362">
+      <c r="O131" s="363">
         <f>SUM(M131:M133)</f>
         <v>176.06</v>
       </c>
-      <c r="P131" s="359"/>
+      <c r="P131" s="374"/>
     </row>
     <row r="132" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C132">
@@ -14305,9 +14305,9 @@
         <f>(L132+O120)</f>
         <v>81.510000000000005</v>
       </c>
-      <c r="N132" s="363"/>
-      <c r="O132" s="363"/>
-      <c r="P132" s="359"/>
+      <c r="N132" s="364"/>
+      <c r="O132" s="364"/>
+      <c r="P132" s="374"/>
     </row>
     <row r="133" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H133" s="5" t="s">
@@ -14332,9 +14332,9 @@
         <f>(L133+O120)</f>
         <v>22.2</v>
       </c>
-      <c r="N133" s="364"/>
-      <c r="O133" s="364"/>
-      <c r="P133" s="359"/>
+      <c r="N133" s="365"/>
+      <c r="O133" s="365"/>
+      <c r="P133" s="374"/>
     </row>
     <row r="134" spans="3:16" x14ac:dyDescent="0.25">
       <c r="H134" s="163" t="s">
@@ -14679,12 +14679,12 @@
         <f>SUM(G149:G166)</f>
         <v>7276.4400000000005</v>
       </c>
-      <c r="I149" s="373" t="s">
+      <c r="I149" s="356" t="s">
         <v>1829</v>
       </c>
-      <c r="J149" s="374"/>
-      <c r="K149" s="374"/>
-      <c r="L149" s="374"/>
+      <c r="J149" s="357"/>
+      <c r="K149" s="357"/>
+      <c r="L149" s="357"/>
       <c r="M149" s="156">
         <v>85</v>
       </c>
@@ -14699,10 +14699,10 @@
       </c>
       <c r="G150" s="5"/>
       <c r="H150" s="5"/>
-      <c r="I150" s="374"/>
-      <c r="J150" s="374"/>
-      <c r="K150" s="374"/>
-      <c r="L150" s="374"/>
+      <c r="I150" s="357"/>
+      <c r="J150" s="357"/>
+      <c r="K150" s="357"/>
+      <c r="L150" s="357"/>
       <c r="M150" s="156"/>
       <c r="N150" s="156"/>
       <c r="O150" s="156"/>
@@ -14721,10 +14721,10 @@
         <f>ROUND(-G151/G149*100,2)</f>
         <v>10.07</v>
       </c>
-      <c r="I151" s="374"/>
-      <c r="J151" s="374"/>
-      <c r="K151" s="374"/>
-      <c r="L151" s="374"/>
+      <c r="I151" s="357"/>
+      <c r="J151" s="357"/>
+      <c r="K151" s="357"/>
+      <c r="L151" s="357"/>
       <c r="M151" s="156"/>
       <c r="N151" s="156"/>
       <c r="O151" s="156"/>
@@ -14743,10 +14743,10 @@
         <f>ROUND((G152/G149)*100,2)</f>
         <v>-6.33</v>
       </c>
-      <c r="I152" s="374"/>
-      <c r="J152" s="374"/>
-      <c r="K152" s="374"/>
-      <c r="L152" s="374"/>
+      <c r="I152" s="357"/>
+      <c r="J152" s="357"/>
+      <c r="K152" s="357"/>
+      <c r="L152" s="357"/>
       <c r="M152" s="156"/>
       <c r="N152" s="156"/>
       <c r="O152" s="156"/>
@@ -14765,10 +14765,10 @@
         <f>ROUND((G153/G149)*100,2)</f>
         <v>-1.48</v>
       </c>
-      <c r="I153" s="374"/>
-      <c r="J153" s="374"/>
-      <c r="K153" s="374"/>
-      <c r="L153" s="374"/>
+      <c r="I153" s="357"/>
+      <c r="J153" s="357"/>
+      <c r="K153" s="357"/>
+      <c r="L153" s="357"/>
       <c r="M153" s="156"/>
       <c r="N153" s="156"/>
       <c r="O153" s="156"/>
@@ -14787,10 +14787,10 @@
         <f>ROUND((-G154/G149)*100,2)</f>
         <v>3.36</v>
       </c>
-      <c r="I154" s="374"/>
-      <c r="J154" s="374"/>
-      <c r="K154" s="374"/>
-      <c r="L154" s="374"/>
+      <c r="I154" s="357"/>
+      <c r="J154" s="357"/>
+      <c r="K154" s="357"/>
+      <c r="L154" s="357"/>
       <c r="M154" s="156"/>
       <c r="N154" s="156"/>
       <c r="O154" s="156"/>
@@ -14800,10 +14800,10 @@
       <c r="E155" s="155"/>
       <c r="F155" s="5"/>
       <c r="G155" s="5"/>
-      <c r="I155" s="374"/>
-      <c r="J155" s="374"/>
-      <c r="K155" s="374"/>
-      <c r="L155" s="374"/>
+      <c r="I155" s="357"/>
+      <c r="J155" s="357"/>
+      <c r="K155" s="357"/>
+      <c r="L155" s="357"/>
       <c r="M155" s="345"/>
       <c r="N155" s="346" t="s">
         <v>1984</v>
@@ -14828,10 +14828,10 @@
         <f>ROUND((-G156/G149)*100,2)</f>
         <v>6</v>
       </c>
-      <c r="I156" s="374"/>
-      <c r="J156" s="374"/>
-      <c r="K156" s="374"/>
-      <c r="L156" s="374"/>
+      <c r="I156" s="357"/>
+      <c r="J156" s="357"/>
+      <c r="K156" s="357"/>
+      <c r="L156" s="357"/>
       <c r="M156" s="345" t="s">
         <v>1419</v>
       </c>
@@ -14857,10 +14857,10 @@
         <f>ROUND((-G157/G149)*100,2)</f>
         <v>0</v>
       </c>
-      <c r="I157" s="374"/>
-      <c r="J157" s="374"/>
-      <c r="K157" s="374"/>
-      <c r="L157" s="374"/>
+      <c r="I157" s="357"/>
+      <c r="J157" s="357"/>
+      <c r="K157" s="357"/>
+      <c r="L157" s="357"/>
       <c r="M157" s="345" t="s">
         <v>1417</v>
       </c>
@@ -14886,10 +14886,10 @@
         <f>ROUND((-G158/G149)*100,2)</f>
         <v>0</v>
       </c>
-      <c r="I158" s="374"/>
-      <c r="J158" s="374"/>
-      <c r="K158" s="374"/>
-      <c r="L158" s="374"/>
+      <c r="I158" s="357"/>
+      <c r="J158" s="357"/>
+      <c r="K158" s="357"/>
+      <c r="L158" s="357"/>
       <c r="M158" s="345" t="s">
         <v>1416</v>
       </c>
@@ -14910,10 +14910,10 @@
       <c r="F159" s="155"/>
       <c r="G159" s="155"/>
       <c r="H159" s="156"/>
-      <c r="I159" s="374"/>
-      <c r="J159" s="374"/>
-      <c r="K159" s="374"/>
-      <c r="L159" s="374"/>
+      <c r="I159" s="357"/>
+      <c r="J159" s="357"/>
+      <c r="K159" s="357"/>
+      <c r="L159" s="357"/>
       <c r="M159" s="345" t="s">
         <v>1429</v>
       </c>
@@ -14934,10 +14934,10 @@
       <c r="F160" s="155"/>
       <c r="G160" s="155"/>
       <c r="H160" s="156"/>
-      <c r="I160" s="374"/>
-      <c r="J160" s="374"/>
-      <c r="K160" s="374"/>
-      <c r="L160" s="374"/>
+      <c r="I160" s="357"/>
+      <c r="J160" s="357"/>
+      <c r="K160" s="357"/>
+      <c r="L160" s="357"/>
       <c r="M160" s="156"/>
       <c r="N160" s="156"/>
       <c r="O160" s="156"/>
@@ -14948,10 +14948,10 @@
       <c r="F161" s="155"/>
       <c r="G161" s="155"/>
       <c r="H161" s="156"/>
-      <c r="I161" s="374"/>
-      <c r="J161" s="374"/>
-      <c r="K161" s="374"/>
-      <c r="L161" s="374"/>
+      <c r="I161" s="357"/>
+      <c r="J161" s="357"/>
+      <c r="K161" s="357"/>
+      <c r="L161" s="357"/>
       <c r="M161" s="156"/>
       <c r="N161" s="156"/>
       <c r="O161" s="156"/>
@@ -14962,10 +14962,10 @@
       <c r="F162" s="155"/>
       <c r="G162" s="155"/>
       <c r="H162" s="156"/>
-      <c r="I162" s="374"/>
-      <c r="J162" s="374"/>
-      <c r="K162" s="374"/>
-      <c r="L162" s="374"/>
+      <c r="I162" s="357"/>
+      <c r="J162" s="357"/>
+      <c r="K162" s="357"/>
+      <c r="L162" s="357"/>
       <c r="M162" s="156"/>
       <c r="N162" s="156"/>
       <c r="O162" s="156"/>
@@ -14975,10 +14975,10 @@
       <c r="E163" s="155"/>
       <c r="F163" s="155"/>
       <c r="G163" s="155"/>
-      <c r="I163" s="374"/>
-      <c r="J163" s="374"/>
-      <c r="K163" s="374"/>
-      <c r="L163" s="374"/>
+      <c r="I163" s="357"/>
+      <c r="J163" s="357"/>
+      <c r="K163" s="357"/>
+      <c r="L163" s="357"/>
     </row>
     <row r="169" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F169" s="315">
@@ -15369,13 +15369,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="I149:L163"/>
-    <mergeCell ref="N124:N126"/>
-    <mergeCell ref="N127:N128"/>
-    <mergeCell ref="N131:N133"/>
-    <mergeCell ref="D117:F117"/>
-    <mergeCell ref="G117:H117"/>
-    <mergeCell ref="K117:M117"/>
     <mergeCell ref="O124:O126"/>
     <mergeCell ref="P124:P133"/>
     <mergeCell ref="O127:O128"/>
@@ -15386,6 +15379,13 @@
     <mergeCell ref="D116:F116"/>
     <mergeCell ref="G116:H116"/>
     <mergeCell ref="K116:M116"/>
+    <mergeCell ref="I149:L163"/>
+    <mergeCell ref="N124:N126"/>
+    <mergeCell ref="N127:N128"/>
+    <mergeCell ref="N131:N133"/>
+    <mergeCell ref="D117:F117"/>
+    <mergeCell ref="G117:H117"/>
+    <mergeCell ref="K117:M117"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="30" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -21091,18 +21091,18 @@
     <row r="2" spans="4:20" ht="21" x14ac:dyDescent="0.35">
       <c r="E2" s="266">
         <f ca="1">TODAY()</f>
-        <v>43293</v>
+        <v>43294</v>
       </c>
       <c r="F2" s="266">
         <v>43621</v>
       </c>
       <c r="G2" s="267">
         <f ca="1">DATEDIF(E2,F2,"d")</f>
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H2" s="267">
         <f ca="1">(DATEDIF(E2,F2,"d")/7)</f>
-        <v>46.857142857142854</v>
+        <v>46.714285714285715</v>
       </c>
       <c r="I2" s="267">
         <f ca="1">DATEDIF(E2,F2,"m")</f>
@@ -22403,22 +22403,22 @@
       <c r="N64" s="312"/>
     </row>
     <row r="65" spans="2:22" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B65" s="365" t="s">
+      <c r="B65" s="375" t="s">
         <v>1934</v>
       </c>
-      <c r="C65" s="366"/>
-      <c r="F65" s="365" t="s">
+      <c r="C65" s="376"/>
+      <c r="F65" s="375" t="s">
         <v>1780</v>
       </c>
-      <c r="G65" s="366"/>
+      <c r="G65" s="376"/>
       <c r="H65" s="230">
         <f>SUM(G66:G91)</f>
         <v>3439</v>
       </c>
-      <c r="J65" s="365">
+      <c r="J65" s="375">
         <v>43252</v>
       </c>
-      <c r="K65" s="366"/>
+      <c r="K65" s="376"/>
       <c r="L65" s="265">
         <f>SUM(K66:K91)</f>
         <v>1730</v>
@@ -23830,41 +23830,41 @@
     </row>
     <row r="116" spans="3:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C116" s="245"/>
-      <c r="D116" s="367" t="s">
+      <c r="D116" s="377" t="s">
         <v>1221</v>
       </c>
-      <c r="E116" s="368"/>
-      <c r="F116" s="369"/>
-      <c r="G116" s="370" t="s">
+      <c r="E116" s="378"/>
+      <c r="F116" s="379"/>
+      <c r="G116" s="380" t="s">
         <v>1565</v>
       </c>
-      <c r="H116" s="371"/>
+      <c r="H116" s="381"/>
       <c r="I116" s="199" t="s">
         <v>1566</v>
       </c>
       <c r="J116" s="199" t="s">
         <v>1567</v>
       </c>
-      <c r="K116" s="370" t="s">
+      <c r="K116" s="380" t="s">
         <v>1625</v>
       </c>
-      <c r="L116" s="372"/>
-      <c r="M116" s="371"/>
+      <c r="L116" s="382"/>
+      <c r="M116" s="381"/>
       <c r="N116" s="343"/>
     </row>
     <row r="117" spans="3:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C117" s="245"/>
-      <c r="D117" s="375">
+      <c r="D117" s="366">
         <f>SUM(D115:F115)</f>
         <v>137.57999999999998</v>
       </c>
-      <c r="E117" s="376"/>
-      <c r="F117" s="377"/>
-      <c r="G117" s="378">
+      <c r="E117" s="367"/>
+      <c r="F117" s="368"/>
+      <c r="G117" s="369">
         <f>SUM(G115:H115)</f>
         <v>97.72</v>
       </c>
-      <c r="H117" s="379"/>
+      <c r="H117" s="370"/>
       <c r="I117" s="200">
         <f>SUM(I104:I113)</f>
         <v>59.129999999999995</v>
@@ -23873,12 +23873,12 @@
         <f>SUM(J104:J113)</f>
         <v>71.55</v>
       </c>
-      <c r="K117" s="380">
+      <c r="K117" s="371">
         <f>SUM(K115:M115)</f>
         <v>162.44000000000003</v>
       </c>
-      <c r="L117" s="381"/>
-      <c r="M117" s="382"/>
+      <c r="L117" s="372"/>
+      <c r="M117" s="373"/>
       <c r="N117" s="344"/>
       <c r="O117" s="1">
         <f>(O115-O103)</f>
@@ -23991,14 +23991,14 @@
         <f>(L124+O120)</f>
         <v>62.36</v>
       </c>
-      <c r="N124" s="356" t="s">
+      <c r="N124" s="358" t="s">
         <v>1221</v>
       </c>
-      <c r="O124" s="356">
+      <c r="O124" s="358">
         <f>SUM(M124:M126)</f>
         <v>139.06</v>
       </c>
-      <c r="P124" s="359">
+      <c r="P124" s="374">
         <f>ROUND(SUM(O124:O133),2)</f>
         <v>574.53</v>
       </c>
@@ -24032,9 +24032,9 @@
         <f>(L125+O120)</f>
         <v>59.66</v>
       </c>
-      <c r="N125" s="357"/>
-      <c r="O125" s="357"/>
-      <c r="P125" s="359"/>
+      <c r="N125" s="359"/>
+      <c r="O125" s="359"/>
+      <c r="P125" s="374"/>
     </row>
     <row r="126" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C126" t="s">
@@ -24069,9 +24069,9 @@
         <f>(L126+O120)</f>
         <v>17.04</v>
       </c>
-      <c r="N126" s="358"/>
-      <c r="O126" s="358"/>
-      <c r="P126" s="359"/>
+      <c r="N126" s="360"/>
+      <c r="O126" s="360"/>
+      <c r="P126" s="374"/>
     </row>
     <row r="127" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H127" s="5" t="s">
@@ -24096,14 +24096,14 @@
         <f>(L127+O120)</f>
         <v>62.36</v>
       </c>
-      <c r="N127" s="360" t="s">
+      <c r="N127" s="361" t="s">
         <v>1565</v>
       </c>
-      <c r="O127" s="360">
+      <c r="O127" s="361">
         <f>SUM(M127:M128)</f>
         <v>98.789999999999992</v>
       </c>
-      <c r="P127" s="359"/>
+      <c r="P127" s="374"/>
     </row>
     <row r="128" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H128" s="5" t="s">
@@ -24127,9 +24127,9 @@
         <f>L128</f>
         <v>36.43</v>
       </c>
-      <c r="N128" s="361"/>
-      <c r="O128" s="361"/>
-      <c r="P128" s="359"/>
+      <c r="N128" s="362"/>
+      <c r="O128" s="362"/>
+      <c r="P128" s="374"/>
     </row>
     <row r="129" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H129" s="5" t="s">
@@ -24161,7 +24161,7 @@
         <f>M129</f>
         <v>59.66</v>
       </c>
-      <c r="P129" s="359"/>
+      <c r="P129" s="374"/>
     </row>
     <row r="130" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H130" s="5" t="s">
@@ -24193,7 +24193,7 @@
         <f>M130</f>
         <v>72.210000000000008</v>
       </c>
-      <c r="P130" s="359"/>
+      <c r="P130" s="374"/>
     </row>
     <row r="131" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C131">
@@ -24222,14 +24222,14 @@
         <f>(L131+O120)</f>
         <v>109.47</v>
       </c>
-      <c r="N131" s="362" t="s">
+      <c r="N131" s="363" t="s">
         <v>1983</v>
       </c>
-      <c r="O131" s="362">
+      <c r="O131" s="363">
         <f>SUM(M131:M133)</f>
         <v>204.81</v>
       </c>
-      <c r="P131" s="359"/>
+      <c r="P131" s="374"/>
     </row>
     <row r="132" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C132">
@@ -24258,9 +24258,9 @@
         <f>(L132+O120)</f>
         <v>78.300000000000011</v>
       </c>
-      <c r="N132" s="363"/>
-      <c r="O132" s="363"/>
-      <c r="P132" s="359"/>
+      <c r="N132" s="364"/>
+      <c r="O132" s="364"/>
+      <c r="P132" s="374"/>
     </row>
     <row r="133" spans="3:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H133" s="5" t="s">
@@ -24285,9 +24285,9 @@
         <f>(L133+O120)</f>
         <v>17.04</v>
       </c>
-      <c r="N133" s="364"/>
-      <c r="O133" s="364"/>
-      <c r="P133" s="359"/>
+      <c r="N133" s="365"/>
+      <c r="O133" s="365"/>
+      <c r="P133" s="374"/>
     </row>
     <row r="134" spans="3:16" x14ac:dyDescent="0.25">
       <c r="I134">
@@ -24632,12 +24632,12 @@
         <f>SUM(G149:G166)</f>
         <v>7276.4400000000005</v>
       </c>
-      <c r="I149" s="373" t="s">
+      <c r="I149" s="356" t="s">
         <v>1829</v>
       </c>
-      <c r="J149" s="374"/>
-      <c r="K149" s="374"/>
-      <c r="L149" s="374"/>
+      <c r="J149" s="357"/>
+      <c r="K149" s="357"/>
+      <c r="L149" s="357"/>
       <c r="M149" s="156">
         <v>85</v>
       </c>
@@ -24652,10 +24652,10 @@
       </c>
       <c r="G150" s="5"/>
       <c r="H150" s="5"/>
-      <c r="I150" s="374"/>
-      <c r="J150" s="374"/>
-      <c r="K150" s="374"/>
-      <c r="L150" s="374"/>
+      <c r="I150" s="357"/>
+      <c r="J150" s="357"/>
+      <c r="K150" s="357"/>
+      <c r="L150" s="357"/>
       <c r="M150" s="156"/>
       <c r="N150" s="156"/>
       <c r="O150" s="156"/>
@@ -24674,10 +24674,10 @@
         <f>ROUND(-G151/G149*100,2)</f>
         <v>10.07</v>
       </c>
-      <c r="I151" s="374"/>
-      <c r="J151" s="374"/>
-      <c r="K151" s="374"/>
-      <c r="L151" s="374"/>
+      <c r="I151" s="357"/>
+      <c r="J151" s="357"/>
+      <c r="K151" s="357"/>
+      <c r="L151" s="357"/>
       <c r="M151" s="156"/>
       <c r="N151" s="156"/>
       <c r="O151" s="156"/>
@@ -24696,10 +24696,10 @@
         <f>ROUND((G152/G149)*100,2)</f>
         <v>-6.33</v>
       </c>
-      <c r="I152" s="374"/>
-      <c r="J152" s="374"/>
-      <c r="K152" s="374"/>
-      <c r="L152" s="374"/>
+      <c r="I152" s="357"/>
+      <c r="J152" s="357"/>
+      <c r="K152" s="357"/>
+      <c r="L152" s="357"/>
       <c r="M152" s="156"/>
       <c r="N152" s="156"/>
       <c r="O152" s="156"/>
@@ -24718,10 +24718,10 @@
         <f>ROUND((G153/G149)*100,2)</f>
         <v>-1.48</v>
       </c>
-      <c r="I153" s="374"/>
-      <c r="J153" s="374"/>
-      <c r="K153" s="374"/>
-      <c r="L153" s="374"/>
+      <c r="I153" s="357"/>
+      <c r="J153" s="357"/>
+      <c r="K153" s="357"/>
+      <c r="L153" s="357"/>
       <c r="M153" s="156"/>
       <c r="N153" s="156"/>
       <c r="O153" s="156"/>
@@ -24740,10 +24740,10 @@
         <f>ROUND((-G154/G149)*100,2)</f>
         <v>3.36</v>
       </c>
-      <c r="I154" s="374"/>
-      <c r="J154" s="374"/>
-      <c r="K154" s="374"/>
-      <c r="L154" s="374"/>
+      <c r="I154" s="357"/>
+      <c r="J154" s="357"/>
+      <c r="K154" s="357"/>
+      <c r="L154" s="357"/>
       <c r="M154" s="156"/>
       <c r="N154" s="156"/>
       <c r="O154" s="156"/>
@@ -24753,10 +24753,10 @@
       <c r="E155" s="155"/>
       <c r="F155" s="5"/>
       <c r="G155" s="5"/>
-      <c r="I155" s="374"/>
-      <c r="J155" s="374"/>
-      <c r="K155" s="374"/>
-      <c r="L155" s="374"/>
+      <c r="I155" s="357"/>
+      <c r="J155" s="357"/>
+      <c r="K155" s="357"/>
+      <c r="L155" s="357"/>
       <c r="M155" s="156"/>
       <c r="N155" s="156"/>
       <c r="O155" s="156"/>
@@ -24774,10 +24774,10 @@
         <f>ROUND((-G156/G149)*100,2)</f>
         <v>6</v>
       </c>
-      <c r="I156" s="374"/>
-      <c r="J156" s="374"/>
-      <c r="K156" s="374"/>
-      <c r="L156" s="374"/>
+      <c r="I156" s="357"/>
+      <c r="J156" s="357"/>
+      <c r="K156" s="357"/>
+      <c r="L156" s="357"/>
       <c r="M156" s="156"/>
       <c r="N156" s="156"/>
       <c r="O156" s="156"/>
@@ -24793,10 +24793,10 @@
         <f>ROUND((-G157/G149)*100,2)</f>
         <v>0</v>
       </c>
-      <c r="I157" s="374"/>
-      <c r="J157" s="374"/>
-      <c r="K157" s="374"/>
-      <c r="L157" s="374"/>
+      <c r="I157" s="357"/>
+      <c r="J157" s="357"/>
+      <c r="K157" s="357"/>
+      <c r="L157" s="357"/>
       <c r="M157" s="156"/>
       <c r="N157" s="156"/>
       <c r="O157" s="156"/>
@@ -24812,10 +24812,10 @@
         <f>ROUND((-G158/G149)*100,2)</f>
         <v>0</v>
       </c>
-      <c r="I158" s="374"/>
-      <c r="J158" s="374"/>
-      <c r="K158" s="374"/>
-      <c r="L158" s="374"/>
+      <c r="I158" s="357"/>
+      <c r="J158" s="357"/>
+      <c r="K158" s="357"/>
+      <c r="L158" s="357"/>
       <c r="M158" s="156"/>
       <c r="N158" s="156"/>
       <c r="O158" s="156"/>
@@ -24826,10 +24826,10 @@
       <c r="F159" s="155"/>
       <c r="G159" s="155"/>
       <c r="H159" s="156"/>
-      <c r="I159" s="374"/>
-      <c r="J159" s="374"/>
-      <c r="K159" s="374"/>
-      <c r="L159" s="374"/>
+      <c r="I159" s="357"/>
+      <c r="J159" s="357"/>
+      <c r="K159" s="357"/>
+      <c r="L159" s="357"/>
       <c r="M159" s="156"/>
       <c r="N159" s="156"/>
       <c r="O159" s="156"/>
@@ -24840,10 +24840,10 @@
       <c r="F160" s="155"/>
       <c r="G160" s="155"/>
       <c r="H160" s="156"/>
-      <c r="I160" s="374"/>
-      <c r="J160" s="374"/>
-      <c r="K160" s="374"/>
-      <c r="L160" s="374"/>
+      <c r="I160" s="357"/>
+      <c r="J160" s="357"/>
+      <c r="K160" s="357"/>
+      <c r="L160" s="357"/>
       <c r="M160" s="156"/>
       <c r="N160" s="156"/>
       <c r="O160" s="156"/>
@@ -24854,10 +24854,10 @@
       <c r="F161" s="155"/>
       <c r="G161" s="155"/>
       <c r="H161" s="156"/>
-      <c r="I161" s="374"/>
-      <c r="J161" s="374"/>
-      <c r="K161" s="374"/>
-      <c r="L161" s="374"/>
+      <c r="I161" s="357"/>
+      <c r="J161" s="357"/>
+      <c r="K161" s="357"/>
+      <c r="L161" s="357"/>
       <c r="M161" s="156"/>
       <c r="N161" s="156"/>
       <c r="O161" s="156"/>
@@ -24868,10 +24868,10 @@
       <c r="F162" s="155"/>
       <c r="G162" s="155"/>
       <c r="H162" s="156"/>
-      <c r="I162" s="374"/>
-      <c r="J162" s="374"/>
-      <c r="K162" s="374"/>
-      <c r="L162" s="374"/>
+      <c r="I162" s="357"/>
+      <c r="J162" s="357"/>
+      <c r="K162" s="357"/>
+      <c r="L162" s="357"/>
       <c r="M162" s="156"/>
       <c r="N162" s="156"/>
       <c r="O162" s="156"/>
@@ -24881,10 +24881,10 @@
       <c r="E163" s="155"/>
       <c r="F163" s="155"/>
       <c r="G163" s="155"/>
-      <c r="I163" s="374"/>
-      <c r="J163" s="374"/>
-      <c r="K163" s="374"/>
-      <c r="L163" s="374"/>
+      <c r="I163" s="357"/>
+      <c r="J163" s="357"/>
+      <c r="K163" s="357"/>
+      <c r="L163" s="357"/>
     </row>
     <row r="180" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H180" s="5">
@@ -25052,13 +25052,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="I149:L163"/>
-    <mergeCell ref="N124:N126"/>
-    <mergeCell ref="N127:N128"/>
-    <mergeCell ref="N131:N133"/>
-    <mergeCell ref="D117:F117"/>
-    <mergeCell ref="G117:H117"/>
-    <mergeCell ref="K117:M117"/>
     <mergeCell ref="O124:O126"/>
     <mergeCell ref="P124:P133"/>
     <mergeCell ref="O127:O128"/>
@@ -25069,6 +25062,13 @@
     <mergeCell ref="D116:F116"/>
     <mergeCell ref="G116:H116"/>
     <mergeCell ref="K116:M116"/>
+    <mergeCell ref="I149:L163"/>
+    <mergeCell ref="N124:N126"/>
+    <mergeCell ref="N127:N128"/>
+    <mergeCell ref="N131:N133"/>
+    <mergeCell ref="D117:F117"/>
+    <mergeCell ref="G117:H117"/>
+    <mergeCell ref="K117:M117"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="30" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -25105,64 +25105,64 @@
       <c r="C4" t="s">
         <v>177</v>
       </c>
-      <c r="H4" s="373" t="s">
+      <c r="H4" s="356" t="s">
         <v>186</v>
       </c>
-      <c r="I4" s="373"/>
-      <c r="J4" s="373"/>
-      <c r="K4" s="373"/>
-      <c r="L4" s="373"/>
-      <c r="M4" s="373"/>
-      <c r="N4" s="373"/>
+      <c r="I4" s="356"/>
+      <c r="J4" s="356"/>
+      <c r="K4" s="356"/>
+      <c r="L4" s="356"/>
+      <c r="M4" s="356"/>
+      <c r="N4" s="356"/>
       <c r="O4" s="15"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>178</v>
       </c>
-      <c r="H5" s="373"/>
-      <c r="I5" s="373"/>
-      <c r="J5" s="373"/>
-      <c r="K5" s="373"/>
-      <c r="L5" s="373"/>
-      <c r="M5" s="373"/>
-      <c r="N5" s="373"/>
+      <c r="H5" s="356"/>
+      <c r="I5" s="356"/>
+      <c r="J5" s="356"/>
+      <c r="K5" s="356"/>
+      <c r="L5" s="356"/>
+      <c r="M5" s="356"/>
+      <c r="N5" s="356"/>
       <c r="O5" s="15"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>179</v>
       </c>
-      <c r="H6" s="373"/>
-      <c r="I6" s="373"/>
-      <c r="J6" s="373"/>
-      <c r="K6" s="373"/>
-      <c r="L6" s="373"/>
-      <c r="M6" s="373"/>
-      <c r="N6" s="373"/>
+      <c r="H6" s="356"/>
+      <c r="I6" s="356"/>
+      <c r="J6" s="356"/>
+      <c r="K6" s="356"/>
+      <c r="L6" s="356"/>
+      <c r="M6" s="356"/>
+      <c r="N6" s="356"/>
       <c r="O6" s="15"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>181</v>
       </c>
-      <c r="H7" s="373"/>
-      <c r="I7" s="373"/>
-      <c r="J7" s="373"/>
-      <c r="K7" s="373"/>
-      <c r="L7" s="373"/>
-      <c r="M7" s="373"/>
-      <c r="N7" s="373"/>
+      <c r="H7" s="356"/>
+      <c r="I7" s="356"/>
+      <c r="J7" s="356"/>
+      <c r="K7" s="356"/>
+      <c r="L7" s="356"/>
+      <c r="M7" s="356"/>
+      <c r="N7" s="356"/>
       <c r="O7" s="15"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H8" s="373"/>
-      <c r="I8" s="373"/>
-      <c r="J8" s="373"/>
-      <c r="K8" s="373"/>
-      <c r="L8" s="373"/>
-      <c r="M8" s="373"/>
-      <c r="N8" s="373"/>
+      <c r="H8" s="356"/>
+      <c r="I8" s="356"/>
+      <c r="J8" s="356"/>
+      <c r="K8" s="356"/>
+      <c r="L8" s="356"/>
+      <c r="M8" s="356"/>
+      <c r="N8" s="356"/>
       <c r="O8" s="15"/>
       <c r="P8" s="17" t="s">
         <v>182</v>
@@ -25172,13 +25172,13 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H9" s="373"/>
-      <c r="I9" s="373"/>
-      <c r="J9" s="373"/>
-      <c r="K9" s="373"/>
-      <c r="L9" s="373"/>
-      <c r="M9" s="373"/>
-      <c r="N9" s="373"/>
+      <c r="H9" s="356"/>
+      <c r="I9" s="356"/>
+      <c r="J9" s="356"/>
+      <c r="K9" s="356"/>
+      <c r="L9" s="356"/>
+      <c r="M9" s="356"/>
+      <c r="N9" s="356"/>
       <c r="O9" s="15" t="s">
         <v>191</v>
       </c>
@@ -25193,13 +25193,13 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H10" s="373"/>
-      <c r="I10" s="373"/>
-      <c r="J10" s="373"/>
-      <c r="K10" s="373"/>
-      <c r="L10" s="373"/>
-      <c r="M10" s="373"/>
-      <c r="N10" s="373"/>
+      <c r="H10" s="356"/>
+      <c r="I10" s="356"/>
+      <c r="J10" s="356"/>
+      <c r="K10" s="356"/>
+      <c r="L10" s="356"/>
+      <c r="M10" s="356"/>
+      <c r="N10" s="356"/>
       <c r="O10" s="15" t="s">
         <v>185</v>
       </c>
@@ -25214,13 +25214,13 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H11" s="373"/>
-      <c r="I11" s="373"/>
-      <c r="J11" s="373"/>
-      <c r="K11" s="373"/>
-      <c r="L11" s="373"/>
-      <c r="M11" s="373"/>
-      <c r="N11" s="373"/>
+      <c r="H11" s="356"/>
+      <c r="I11" s="356"/>
+      <c r="J11" s="356"/>
+      <c r="K11" s="356"/>
+      <c r="L11" s="356"/>
+      <c r="M11" s="356"/>
+      <c r="N11" s="356"/>
       <c r="O11" s="15"/>
       <c r="P11" s="18"/>
       <c r="Q11" s="20">
@@ -25231,13 +25231,13 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H12" s="373"/>
-      <c r="I12" s="373"/>
-      <c r="J12" s="373"/>
-      <c r="K12" s="373"/>
-      <c r="L12" s="373"/>
-      <c r="M12" s="373"/>
-      <c r="N12" s="373"/>
+      <c r="H12" s="356"/>
+      <c r="I12" s="356"/>
+      <c r="J12" s="356"/>
+      <c r="K12" s="356"/>
+      <c r="L12" s="356"/>
+      <c r="M12" s="356"/>
+      <c r="N12" s="356"/>
       <c r="O12" s="15"/>
       <c r="P12" s="18"/>
       <c r="Q12" s="20">
@@ -25254,13 +25254,13 @@
       <c r="D13" t="s">
         <v>183</v>
       </c>
-      <c r="H13" s="373"/>
-      <c r="I13" s="373"/>
-      <c r="J13" s="373"/>
-      <c r="K13" s="373"/>
-      <c r="L13" s="373"/>
-      <c r="M13" s="373"/>
-      <c r="N13" s="373"/>
+      <c r="H13" s="356"/>
+      <c r="I13" s="356"/>
+      <c r="J13" s="356"/>
+      <c r="K13" s="356"/>
+      <c r="L13" s="356"/>
+      <c r="M13" s="356"/>
+      <c r="N13" s="356"/>
       <c r="O13" s="15"/>
       <c r="P13" s="18"/>
       <c r="Q13" s="20">
@@ -25280,13 +25280,13 @@
       <c r="C14">
         <v>2577</v>
       </c>
-      <c r="H14" s="373"/>
-      <c r="I14" s="373"/>
-      <c r="J14" s="373"/>
-      <c r="K14" s="373"/>
-      <c r="L14" s="373"/>
-      <c r="M14" s="373"/>
-      <c r="N14" s="373"/>
+      <c r="H14" s="356"/>
+      <c r="I14" s="356"/>
+      <c r="J14" s="356"/>
+      <c r="K14" s="356"/>
+      <c r="L14" s="356"/>
+      <c r="M14" s="356"/>
+      <c r="N14" s="356"/>
       <c r="O14" s="15"/>
       <c r="P14" s="18"/>
       <c r="Q14" s="20">
@@ -25303,49 +25303,49 @@
       <c r="C15">
         <v>5584</v>
       </c>
-      <c r="H15" s="373"/>
-      <c r="I15" s="373"/>
-      <c r="J15" s="373"/>
-      <c r="K15" s="373"/>
-      <c r="L15" s="373"/>
-      <c r="M15" s="373"/>
-      <c r="N15" s="373"/>
+      <c r="H15" s="356"/>
+      <c r="I15" s="356"/>
+      <c r="J15" s="356"/>
+      <c r="K15" s="356"/>
+      <c r="L15" s="356"/>
+      <c r="M15" s="356"/>
+      <c r="N15" s="356"/>
       <c r="O15" s="15"/>
       <c r="P15" s="18"/>
       <c r="Q15" s="20"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H16" s="373"/>
-      <c r="I16" s="373"/>
-      <c r="J16" s="373"/>
-      <c r="K16" s="373"/>
-      <c r="L16" s="373"/>
-      <c r="M16" s="373"/>
-      <c r="N16" s="373"/>
+      <c r="H16" s="356"/>
+      <c r="I16" s="356"/>
+      <c r="J16" s="356"/>
+      <c r="K16" s="356"/>
+      <c r="L16" s="356"/>
+      <c r="M16" s="356"/>
+      <c r="N16" s="356"/>
       <c r="O16" s="15"/>
       <c r="P16" s="18"/>
       <c r="Q16" s="20"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="H17" s="373"/>
-      <c r="I17" s="373"/>
-      <c r="J17" s="373"/>
-      <c r="K17" s="373"/>
-      <c r="L17" s="373"/>
-      <c r="M17" s="373"/>
-      <c r="N17" s="373"/>
+      <c r="H17" s="356"/>
+      <c r="I17" s="356"/>
+      <c r="J17" s="356"/>
+      <c r="K17" s="356"/>
+      <c r="L17" s="356"/>
+      <c r="M17" s="356"/>
+      <c r="N17" s="356"/>
       <c r="O17" s="15"/>
       <c r="P17" s="18"/>
       <c r="Q17" s="20"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="H18" s="373"/>
-      <c r="I18" s="373"/>
-      <c r="J18" s="373"/>
-      <c r="K18" s="373"/>
-      <c r="L18" s="373"/>
-      <c r="M18" s="373"/>
-      <c r="N18" s="373"/>
+      <c r="H18" s="356"/>
+      <c r="I18" s="356"/>
+      <c r="J18" s="356"/>
+      <c r="K18" s="356"/>
+      <c r="L18" s="356"/>
+      <c r="M18" s="356"/>
+      <c r="N18" s="356"/>
       <c r="O18" s="15"/>
       <c r="P18" s="18"/>
       <c r="Q18" s="20"/>
@@ -28153,7 +28153,7 @@
       <c r="B2" t="s">
         <v>623</v>
       </c>
-      <c r="C2" s="373" t="s">
+      <c r="C2" s="356" t="s">
         <v>626</v>
       </c>
       <c r="I2">
@@ -28173,7 +28173,7 @@
       <c r="B3" t="s">
         <v>624</v>
       </c>
-      <c r="C3" s="373"/>
+      <c r="C3" s="356"/>
       <c r="F3" t="s">
         <v>698</v>
       </c>
@@ -28195,7 +28195,7 @@
       <c r="B4" t="s">
         <v>625</v>
       </c>
-      <c r="C4" s="373"/>
+      <c r="C4" s="356"/>
       <c r="F4" t="s">
         <v>699</v>
       </c>
@@ -31401,10 +31401,10 @@
       <c r="D13" s="209" t="s">
         <v>1635</v>
       </c>
-      <c r="E13" s="416" t="s">
+      <c r="E13" s="401" t="s">
         <v>1654</v>
       </c>
-      <c r="F13" s="417"/>
+      <c r="F13" s="402"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="206" t="s">
@@ -31413,40 +31413,40 @@
       <c r="D14" s="209" t="s">
         <v>1636</v>
       </c>
-      <c r="E14" s="418" t="s">
+      <c r="E14" s="403" t="s">
         <v>1651</v>
       </c>
-      <c r="F14" s="419"/>
+      <c r="F14" s="404"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="207"/>
       <c r="D15" s="209" t="s">
         <v>1638</v>
       </c>
-      <c r="E15" s="408" t="s">
+      <c r="E15" s="405" t="s">
         <v>1652</v>
       </c>
-      <c r="F15" s="409"/>
+      <c r="F15" s="406"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="207"/>
       <c r="D16" s="209" t="s">
         <v>1639</v>
       </c>
-      <c r="E16" s="408" t="s">
+      <c r="E16" s="405" t="s">
         <v>1653</v>
       </c>
-      <c r="F16" s="409"/>
+      <c r="F16" s="406"/>
     </row>
     <row r="17" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="207"/>
       <c r="D17" s="209" t="s">
         <v>1640</v>
       </c>
-      <c r="E17" s="408" t="s">
+      <c r="E17" s="405" t="s">
         <v>1655</v>
       </c>
-      <c r="F17" s="409"/>
+      <c r="F17" s="406"/>
     </row>
     <row r="18" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="207"/>
@@ -31463,111 +31463,111 @@
       <c r="D19" s="212" t="s">
         <v>1643</v>
       </c>
-      <c r="E19" s="414" t="s">
+      <c r="E19" s="399" t="s">
         <v>1656</v>
       </c>
-      <c r="F19" s="415"/>
+      <c r="F19" s="400"/>
     </row>
     <row r="20" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="208"/>
       <c r="D20" s="209" t="s">
         <v>1644</v>
       </c>
-      <c r="E20" s="401" t="s">
+      <c r="E20" s="409" t="s">
         <v>1657</v>
       </c>
-      <c r="F20" s="402"/>
+      <c r="F20" s="410"/>
     </row>
     <row r="21" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="403" t="s">
+      <c r="C21" s="411" t="s">
         <v>1645</v>
       </c>
       <c r="D21" s="209" t="s">
         <v>1635</v>
       </c>
-      <c r="E21" s="406" t="s">
+      <c r="E21" s="414" t="s">
         <v>1646</v>
       </c>
-      <c r="F21" s="407"/>
+      <c r="F21" s="415"/>
     </row>
     <row r="22" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="404"/>
+      <c r="C22" s="412"/>
       <c r="D22" s="209" t="s">
         <v>1636</v>
       </c>
-      <c r="E22" s="408" t="s">
+      <c r="E22" s="405" t="s">
         <v>1637</v>
       </c>
-      <c r="F22" s="409"/>
+      <c r="F22" s="406"/>
     </row>
     <row r="23" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="404"/>
+      <c r="C23" s="412"/>
       <c r="D23" s="209" t="s">
         <v>1638</v>
       </c>
-      <c r="E23" s="408" t="s">
+      <c r="E23" s="405" t="s">
         <v>1647</v>
       </c>
-      <c r="F23" s="409"/>
+      <c r="F23" s="406"/>
     </row>
     <row r="24" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="404"/>
+      <c r="C24" s="412"/>
       <c r="D24" s="209" t="s">
         <v>1639</v>
       </c>
-      <c r="E24" s="408" t="s">
+      <c r="E24" s="405" t="s">
         <v>1648</v>
       </c>
-      <c r="F24" s="409"/>
+      <c r="F24" s="406"/>
     </row>
     <row r="25" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="404"/>
+      <c r="C25" s="412"/>
       <c r="D25" s="209" t="s">
         <v>1640</v>
       </c>
-      <c r="E25" s="408" t="s">
+      <c r="E25" s="405" t="s">
         <v>1649</v>
       </c>
-      <c r="F25" s="409"/>
+      <c r="F25" s="406"/>
     </row>
     <row r="26" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="404"/>
+      <c r="C26" s="412"/>
       <c r="D26" s="209" t="s">
         <v>1641</v>
       </c>
-      <c r="E26" s="408" t="s">
+      <c r="E26" s="405" t="s">
         <v>1642</v>
       </c>
-      <c r="F26" s="409"/>
+      <c r="F26" s="406"/>
     </row>
     <row r="27" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C27" s="404"/>
+      <c r="C27" s="412"/>
       <c r="D27" s="212" t="s">
         <v>1643</v>
       </c>
-      <c r="E27" s="410" t="s">
+      <c r="E27" s="416" t="s">
         <v>1650</v>
       </c>
-      <c r="F27" s="411"/>
+      <c r="F27" s="417"/>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C28" s="404"/>
+      <c r="C28" s="412"/>
       <c r="D28" s="212" t="s">
         <v>1644</v>
       </c>
-      <c r="E28" s="412" t="s">
+      <c r="E28" s="418" t="s">
         <v>1366</v>
       </c>
-      <c r="F28" s="413"/>
+      <c r="F28" s="419"/>
     </row>
     <row r="29" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="404"/>
+      <c r="C29" s="412"/>
       <c r="D29" s="209"/>
-      <c r="E29" s="399"/>
-      <c r="F29" s="400"/>
+      <c r="E29" s="407"/>
+      <c r="F29" s="408"/>
     </row>
     <row r="30" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="405"/>
+      <c r="C30" s="413"/>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
@@ -31645,12 +31645,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="C21:C30"/>
@@ -31662,6 +31656,12 @@
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1"/>

</xml_diff>